<commit_message>
fix(attendance-import): fix import employee
</commit_message>
<xml_diff>
--- a/public/employee_data.xlsx
+++ b/public/employee_data.xlsx
@@ -397,25 +397,72 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
+        <v>comp_code</v>
+      </c>
+      <c r="B1" t="str">
+        <v>branch_code</v>
+      </c>
+      <c r="C1" t="str">
+        <v>nik</v>
+      </c>
+      <c r="D1" t="str">
         <v>name</v>
       </c>
-      <c r="B1" t="str">
+      <c r="E1" t="str">
         <v>first_name</v>
       </c>
-      <c r="C1" t="str">
-        <v>phone</v>
+      <c r="F1" t="str">
+        <v>last_name</v>
+      </c>
+      <c r="G1" t="str">
+        <v>email</v>
+      </c>
+      <c r="H1" t="str">
+        <v>date_in</v>
+      </c>
+      <c r="I1" t="str">
+        <v>date_out</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>C001</v>
+      </c>
+      <c r="B2" t="str">
+        <v>B001</v>
+      </c>
+      <c r="C2" t="str">
+        <v>20240001</v>
+      </c>
+      <c r="D2" t="str">
+        <v>mahar</v>
+      </c>
+      <c r="E2" t="str">
+        <v>mahatma</v>
+      </c>
+      <c r="F2" t="str">
+        <v>mahardhika</v>
+      </c>
+      <c r="G2" t="str">
+        <v>test@test.com</v>
+      </c>
+      <c r="H2" t="str">
+        <v>2024-01-01</v>
+      </c>
+      <c r="I2" t="str">
+        <v>2024-02-02</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:C1"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:I2"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
refactor(sub-division-factory): adjust sub division factory base on new schema
</commit_message>
<xml_diff>
--- a/public/employee_data.xlsx
+++ b/public/employee_data.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:O2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -422,13 +422,31 @@
         <v>last_name</v>
       </c>
       <c r="G1" t="str">
+        <v>phone</v>
+      </c>
+      <c r="H1" t="str">
         <v>email</v>
       </c>
-      <c r="H1" t="str">
+      <c r="I1" t="str">
         <v>date_in</v>
       </c>
-      <c r="I1" t="str">
+      <c r="J1" t="str">
         <v>date_out</v>
+      </c>
+      <c r="K1" t="str">
+        <v>department_code</v>
+      </c>
+      <c r="L1" t="str">
+        <v>division_code</v>
+      </c>
+      <c r="M1" t="str">
+        <v>sub_division_code</v>
+      </c>
+      <c r="N1" t="str">
+        <v>level_code</v>
+      </c>
+      <c r="O1" t="str">
+        <v>position_code</v>
       </c>
     </row>
     <row r="2">
@@ -451,18 +469,21 @@
         <v>mahardhika</v>
       </c>
       <c r="G2" t="str">
+        <v>0879128379</v>
+      </c>
+      <c r="H2" t="str">
         <v>test@test.com</v>
       </c>
-      <c r="H2" t="str">
+      <c r="I2" t="str">
         <v>2024-01-01</v>
       </c>
-      <c r="I2" t="str">
+      <c r="J2" t="str">
         <v>2024-02-02</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:I2"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:O2"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
chore: update ui import user
</commit_message>
<xml_diff>
--- a/public/employee_data.xlsx
+++ b/public/employee_data.xlsx
@@ -404,7 +404,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
-        <v>comp_code</v>
+        <v>company_code</v>
       </c>
       <c r="B1" t="str">
         <v>branch_code</v>
@@ -479,6 +479,21 @@
       </c>
       <c r="J2" t="str">
         <v>2024-02-02</v>
+      </c>
+      <c r="K2" t="str">
+        <v/>
+      </c>
+      <c r="L2" t="str">
+        <v/>
+      </c>
+      <c r="M2" t="str">
+        <v/>
+      </c>
+      <c r="N2" t="str">
+        <v/>
+      </c>
+      <c r="O2" t="str">
+        <v/>
       </c>
     </row>
   </sheetData>

</xml_diff>